<commit_message>
ajout image fond voiture suivant modele
</commit_message>
<xml_diff>
--- a/configuration reglage.xlsx
+++ b/configuration reglage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDUSCMAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90C90C4-1220-4E2A-833F-A22438E7F365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC1EFD6-0A15-4B70-9038-D7DA9B461F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="178">
   <si>
     <t>marque</t>
   </si>
@@ -560,13 +560,19 @@
   </si>
   <si>
     <t>Fenyr SuperSport</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>default_background</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -618,6 +624,12 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -823,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -918,11 +930,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -947,11 +959,17 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="37">
+    <dxf>
+      <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1093,14 +1111,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="Feuille 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="firstRowStripe" dxfId="34"/>
-      <tableStyleElement type="secondRowStripe" dxfId="33"/>
+      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="35"/>
+      <tableStyleElement type="secondRowStripe" dxfId="34"/>
     </tableStyle>
     <tableStyle name="Feuille 2-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="32"/>
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
-      <tableStyleElement type="secondRowStripe" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1115,8 +1133,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="config" displayName="config" ref="A1:AO30">
-  <tableColumns count="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="config" displayName="config" ref="A1:AP30">
+  <tableColumns count="42">
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="car_id"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="rapport_final_min"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="rapport_final_max"/>
@@ -1124,40 +1142,41 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="premiere_vitesse_max"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="deuxieme_vitesse_min"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="deuxieme_vitesse_max"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="troisieme_vitesse_min" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="troisieme_vitesse_max" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="quatrieme_vitesse_min" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="quatrieme_vitesse_max" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="cinquieme_vitesse_min" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="cinquieme_vitesse_max" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="sixieme_vitesse_min" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="sixieme_vitesse_max" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="septieme_vitesse_min" dataDxfId="21"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="septieme_vitesse_max" dataDxfId="20"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="huitieme_vitesse_min" dataDxfId="19"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="huitieme_vitesse_max" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="troisieme_vitesse_min" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="troisieme_vitesse_max" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="quatrieme_vitesse_min" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="quatrieme_vitesse_max" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="cinquieme_vitesse_min" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="cinquieme_vitesse_max" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="sixieme_vitesse_min" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="sixieme_vitesse_max" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="septieme_vitesse_min" dataDxfId="22"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="septieme_vitesse_max" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="huitieme_vitesse_min" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="huitieme_vitesse_max" dataDxfId="19"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="taille_suspension_arriere_min"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="taille_suspension_arriere_max"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="taille_suspension_avant_min"/>
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="taille_suspension_avant_max"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="acceleration_avant_min" dataDxfId="17"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="acceleration_avant_max" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="deceleration_avant_min" dataDxfId="15"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="deceleration_avant_max" dataDxfId="14"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="freinage_avant_min" dataDxfId="13"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="freinage_avant_max" dataDxfId="12"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="distribution_puissance_avant_arriere_min" dataDxfId="11"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="distribution_puissance_avant_arriere_max" dataDxfId="10"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="acceleration_centrale_min" dataDxfId="9"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="acceleration_centrale_max" dataDxfId="8"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="deceleration_centrale_min" dataDxfId="7"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="deceleration_centrale_max" dataDxfId="6"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="freinage_centrale_min" dataDxfId="5"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="freinage_centrale_max" dataDxfId="4"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="pression_pneus_arriere_min" dataDxfId="3"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="pression_pneus_arriere_max" dataDxfId="2"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="pression_pneus_avant_min" dataDxfId="1"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="pression_pneus_avant_max" dataDxfId="0"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="acceleration_avant_min" dataDxfId="18"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="acceleration_avant_max" dataDxfId="17"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="deceleration_avant_min" dataDxfId="16"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="deceleration_avant_max" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="freinage_avant_min" dataDxfId="14"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="freinage_avant_max" dataDxfId="13"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="distribution_puissance_avant_arriere_min" dataDxfId="12"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="distribution_puissance_avant_arriere_max" dataDxfId="11"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="acceleration_centrale_min" dataDxfId="10"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="acceleration_centrale_max" dataDxfId="9"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="deceleration_centrale_min" dataDxfId="8"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="deceleration_centrale_max" dataDxfId="7"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="freinage_centrale_min" dataDxfId="6"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="freinage_centrale_max" dataDxfId="5"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="pression_pneus_arriere_min" dataDxfId="4"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="pression_pneus_arriere_max" dataDxfId="3"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="pression_pneus_avant_min" dataDxfId="2"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="pression_pneus_avant_max" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{8A2977B7-378E-4E7D-9BDC-5DB9009FA432}" name="background" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Feuille 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1415,10 +1434,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AO30"/>
+  <dimension ref="A1:AP30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1:AO1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AP30" sqref="AP30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1429,9 +1448,10 @@
     <col min="16" max="19" width="12.5703125" style="38"/>
     <col min="24" max="40" width="12.5703125" style="38"/>
     <col min="41" max="41" width="28.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="15.75" customHeight="1">
+    <row r="1" spans="1:42" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1555,8 +1575,11 @@
       <c r="AO1" s="39" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" ht="15.75" customHeight="1">
+      <c r="AP1" s="43" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" ht="15.75" customHeight="1">
       <c r="A2" s="11">
         <v>10</v>
       </c>
@@ -1680,8 +1703,11 @@
       <c r="AO2" s="15">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" ht="12.75">
+      <c r="AP2" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" ht="12.75">
       <c r="A3" s="11">
         <v>14</v>
       </c>
@@ -1805,8 +1831,11 @@
       <c r="AO3" s="28">
         <v>9999</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" ht="12.75">
+      <c r="AP3" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" ht="12.75">
       <c r="A4" s="11">
         <v>15</v>
       </c>
@@ -1930,8 +1959,11 @@
       <c r="AO4" s="41">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" ht="12.75">
+      <c r="AP4" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" ht="12.75">
       <c r="A5" s="11">
         <v>20</v>
       </c>
@@ -2049,10 +2081,17 @@
       <c r="AM5" s="27">
         <v>9999</v>
       </c>
-      <c r="AN5" s="29"/>
-      <c r="AO5" s="30"/>
-    </row>
-    <row r="6" spans="1:41" ht="12.75">
+      <c r="AN5" s="29">
+        <v>9999</v>
+      </c>
+      <c r="AO5" s="30">
+        <v>9999</v>
+      </c>
+      <c r="AP5" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" ht="12.75">
       <c r="A6" s="11">
         <v>22</v>
       </c>
@@ -2176,8 +2215,11 @@
       <c r="AO6" s="30">
         <v>9999</v>
       </c>
-    </row>
-    <row r="7" spans="1:41" ht="12.75">
+      <c r="AP6" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" ht="12.75">
       <c r="A7" s="11">
         <v>27</v>
       </c>
@@ -2301,8 +2343,11 @@
       <c r="AO7" s="28">
         <v>9999</v>
       </c>
-    </row>
-    <row r="8" spans="1:41" ht="12.75">
+      <c r="AP7" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" ht="12.75">
       <c r="A8" s="11">
         <v>28</v>
       </c>
@@ -2426,8 +2471,11 @@
       <c r="AO8" s="28">
         <v>9999</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" ht="12.75">
+      <c r="AP8" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" ht="12.75">
       <c r="A9" s="11">
         <v>30</v>
       </c>
@@ -2551,8 +2599,11 @@
       <c r="AO9" s="30">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:41" ht="12.75">
+      <c r="AP9" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" ht="12.75">
       <c r="A10" s="11">
         <v>31</v>
       </c>
@@ -2676,8 +2727,11 @@
       <c r="AO10" s="41">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" ht="12.75">
+      <c r="AP10" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" ht="12.75">
       <c r="A11" s="11">
         <v>32</v>
       </c>
@@ -2801,8 +2855,11 @@
       <c r="AO11" s="30">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" ht="15">
+      <c r="AP11" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" ht="15">
       <c r="A12" s="11">
         <v>36</v>
       </c>
@@ -2926,8 +2983,11 @@
       <c r="AO12" s="15">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:41" ht="15">
+      <c r="AP12" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" ht="15">
       <c r="A13" s="11">
         <v>41</v>
       </c>
@@ -3051,8 +3111,11 @@
       <c r="AO13" s="20">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:41" ht="12.75">
+      <c r="AP13" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" ht="12.75">
       <c r="A14" s="11">
         <v>43</v>
       </c>
@@ -3176,8 +3239,11 @@
       <c r="AO14" s="41">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:41" ht="15">
+      <c r="AP14" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" ht="15">
       <c r="A15" s="11">
         <v>47</v>
       </c>
@@ -3301,8 +3367,11 @@
       <c r="AO15" s="20">
         <v>9999</v>
       </c>
-    </row>
-    <row r="16" spans="1:41" ht="12.75">
+      <c r="AP15" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" ht="12.75">
       <c r="A16" s="11">
         <v>54</v>
       </c>
@@ -3426,8 +3495,11 @@
       <c r="AO16" s="30">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:41" ht="12.75">
+      <c r="AP16" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" ht="12.75">
       <c r="A17" s="11">
         <v>62</v>
       </c>
@@ -3551,8 +3623,11 @@
       <c r="AO17" s="30">
         <v>9999</v>
       </c>
-    </row>
-    <row r="18" spans="1:41" ht="12.75">
+      <c r="AP17" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" ht="12.75">
       <c r="A18" s="11">
         <v>65</v>
       </c>
@@ -3676,8 +3751,11 @@
       <c r="AO18" s="28">
         <v>9999</v>
       </c>
-    </row>
-    <row r="19" spans="1:41" ht="12.75">
+      <c r="AP18" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" ht="12.75">
       <c r="A19" s="11">
         <v>67</v>
       </c>
@@ -3799,8 +3877,11 @@
       <c r="AO19" s="41">
         <v>9999</v>
       </c>
-    </row>
-    <row r="20" spans="1:41" ht="12.75">
+      <c r="AP19" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" ht="12.75">
       <c r="A20" s="11">
         <v>71</v>
       </c>
@@ -3924,8 +4005,11 @@
       <c r="AO20" s="28">
         <v>9999</v>
       </c>
-    </row>
-    <row r="21" spans="1:41" ht="12.75">
+      <c r="AP20" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" ht="12.75">
       <c r="A21" s="11">
         <v>74</v>
       </c>
@@ -4049,8 +4133,11 @@
       <c r="AO21" s="28">
         <v>9999</v>
       </c>
-    </row>
-    <row r="22" spans="1:41" ht="12.75">
+      <c r="AP21" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" ht="12.75">
       <c r="A22" s="11">
         <v>79</v>
       </c>
@@ -4174,8 +4261,11 @@
       <c r="AO22" s="41">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:41" ht="12.75">
+      <c r="AP22" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" ht="12.75">
       <c r="A23" s="11">
         <v>84</v>
       </c>
@@ -4299,8 +4389,11 @@
       <c r="AO23" s="30">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:41" ht="12.75">
+      <c r="AP23" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" ht="12.75">
       <c r="A24" s="11">
         <v>89</v>
       </c>
@@ -4424,8 +4517,11 @@
       <c r="AO24" s="41">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:41" ht="15">
+      <c r="AP24" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" ht="15">
       <c r="A25" s="11">
         <v>90</v>
       </c>
@@ -4549,8 +4645,11 @@
       <c r="AO25" s="15">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:41" ht="12.75">
+      <c r="AP25" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" ht="12.75">
       <c r="A26" s="11">
         <v>91</v>
       </c>
@@ -4674,8 +4773,11 @@
       <c r="AO26" s="42">
         <v>9999</v>
       </c>
-    </row>
-    <row r="27" spans="1:41" ht="15">
+      <c r="AP26" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" ht="15">
       <c r="A27" s="11">
         <v>92</v>
       </c>
@@ -4799,8 +4901,11 @@
       <c r="AO27" s="15">
         <v>9999</v>
       </c>
-    </row>
-    <row r="28" spans="1:41" ht="12.75">
+      <c r="AP27" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" ht="12.75">
       <c r="A28" s="11">
         <v>94</v>
       </c>
@@ -4924,8 +5029,11 @@
       <c r="AO28" s="30">
         <v>9999</v>
       </c>
-    </row>
-    <row r="29" spans="1:41" ht="12.75">
+      <c r="AP28" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" ht="12.75">
       <c r="A29" s="11">
         <v>98</v>
       </c>
@@ -5049,8 +5157,11 @@
       <c r="AO29" s="28">
         <v>9999</v>
       </c>
-    </row>
-    <row r="30" spans="1:41" ht="12.75">
+      <c r="AP29" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" ht="12.75">
       <c r="A30" s="11">
         <v>100</v>
       </c>
@@ -5173,6 +5284,9 @@
       </c>
       <c r="AO30" s="30">
         <v>6</v>
+      </c>
+      <c r="AP30" s="38" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>